<commit_message>
fix to manufacturing files
</commit_message>
<xml_diff>
--- a/vccg/Main/vccg/Manufacturing/vccg_jlcpcb_cpl.xlsx
+++ b/vccg/Main/vccg/Manufacturing/vccg_jlcpcb_cpl.xlsx
@@ -307,7 +307,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -435,7 +435,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,7 +537,7 @@
         <v>6</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,7 +1098,7 @@
         <v>6</v>
       </c>
       <c r="E46" s="0" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,7 +1132,7 @@
         <v>6</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,7 +1149,7 @@
         <v>6</v>
       </c>
       <c r="E49" s="0" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>